<commit_message>
Introduced auto-adjusting histogram bincount for value page
</commit_message>
<xml_diff>
--- a/misc_website_files/RCRwebpagetesting.xlsx
+++ b/misc_website_files/RCRwebpagetesting.xlsx
@@ -1,23 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickk124\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickk124/research/reichart/RCR/RCRRepo/misc_website_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824A32A5-07F4-2F4F-9C69-5978A9A80C5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="7176"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24960" windowHeight="16360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="histogram" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -59,7 +69,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -123,7 +133,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -211,7 +220,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -516,7 +524,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2869,7 +2876,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2899,7 +2912,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2929,7 +2948,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3209,16 +3234,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3253,7 +3278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3303,7 +3328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3348,7 +3373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3384,7 +3409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3420,7 +3445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3456,7 +3481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3492,7 +3517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3519,7 +3544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3555,7 +3580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3591,7 +3616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3620,18 +3645,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C15">
         <f>AVERAGE(A2:A11)</f>
         <v>5.5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -3645,7 +3670,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -3660,7 +3685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2</v>
       </c>
@@ -3675,7 +3700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3</v>
       </c>
@@ -3686,12 +3711,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39">
         <f>AVERAGE(A34:A36)</f>
         <v>2</v>
@@ -3701,4 +3726,3604 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D875F6DD-CF37-204A-894E-FA0426719421}">
+  <dimension ref="A1:A598"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A1:A598"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f t="shared" ref="A2:A65" ca="1" si="0">_xlfn.NORM.INV(RAND(),0,5)</f>
+        <v>-2.467853241413497</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f t="shared" ca="1" si="0"/>
+        <v>-4.7991344904359901</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.9595784352702621</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.0769292700983932</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.0081695724301207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f t="shared" ca="1" si="0"/>
+        <v>-3.971494214468767</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f t="shared" ca="1" si="0"/>
+        <v>-4.3627293559759899</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.89270597248741967</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f t="shared" ca="1" si="0"/>
+        <v>-8.990394853531928</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.7439788941168253</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" ca="1" si="0"/>
+        <v>-2.8101128853571233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.7660550194380624</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f t="shared" ca="1" si="0"/>
+        <v>-3.7994276182323872</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f t="shared" ca="1" si="0"/>
+        <v>-2.5426335089707623</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.8450845502359403</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f t="shared" ca="1" si="0"/>
+        <v>-4.9809543924914204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f t="shared" ca="1" si="0"/>
+        <v>-2.2908779417453524</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <f t="shared" ca="1" si="0"/>
+        <v>13.657972856199327</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.5265629667680596</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <f t="shared" ca="1" si="0"/>
+        <v>8.18020305051866</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <f t="shared" ca="1" si="0"/>
+        <v>12.47029796257455</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.88767304161755</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <f t="shared" ca="1" si="0"/>
+        <v>7.4693638153404809</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.2739041725011702</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.3405417700191045</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.9080894223749558</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <f t="shared" ca="1" si="0"/>
+        <v>6.9059090025819669</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.2691629923147554</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.3528816104496588</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.36477016108110283</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.6778345180673311</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <f t="shared" ca="1" si="0"/>
+        <v>-6.4543331269660886E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <f t="shared" ca="1" si="0"/>
+        <v>-3.5303965875566101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <f t="shared" ca="1" si="0"/>
+        <v>-2.4774526382828945</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <f t="shared" ca="1" si="0"/>
+        <v>-3.3364439526672705</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.2844433061266472E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.32644544755447757</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.1363480130893939</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <f t="shared" ca="1" si="0"/>
+        <v>-4.4342476090212193</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <f t="shared" ca="1" si="0"/>
+        <v>7.5263698380894013</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.45982149667433903</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <f t="shared" ca="1" si="0"/>
+        <v>6.2775833589324144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.6655345411923119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <f t="shared" ca="1" si="0"/>
+        <v>-12.50852354706999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.4940380801997568</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.211514880197202</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.231151659534035</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <f t="shared" ca="1" si="0"/>
+        <v>-7.3116377301256978</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.73077876296164201</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.7201261033724817</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.9691829066841795</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <f t="shared" ca="1" si="0"/>
+        <v>-3.2259032466522819</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <f t="shared" ca="1" si="0"/>
+        <v>-1.0900093590579198</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <f t="shared" ca="1" si="0"/>
+        <v>-2.4681178305593234</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.4780959540226797</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.5184866974455948</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.2121732987879188</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <f t="shared" ca="1" si="0"/>
+        <v>-1.9740038361041328</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.86068991063358313</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <f t="shared" ca="1" si="0"/>
+        <v>-0.82154992317045272</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.21212144448030273</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <f t="shared" ref="A66:A129" ca="1" si="1">_xlfn.NORM.INV(RAND(),0,5)</f>
+        <v>-3.1521373072174641</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.2832909150095757</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.8297602134273849E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.8847760872193255</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <f t="shared" ca="1" si="1"/>
+        <v>-9.3193302192531355</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.48099240965454698</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.505598425461252</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.87862543956674233</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.2258723974623598</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <f t="shared" ca="1" si="1"/>
+        <v>14.379621303223685</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.5730472472672088</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.5089662565227622</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.3953551864622242</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <f t="shared" ca="1" si="1"/>
+        <v>-3.3869899049659091</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.2277403565026771</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <f t="shared" ca="1" si="1"/>
+        <v>-5.4430872677506104</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <f t="shared" ca="1" si="1"/>
+        <v>-1.2017889149249874</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <f t="shared" ca="1" si="1"/>
+        <v>-3.802686624065776</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <f t="shared" ca="1" si="1"/>
+        <v>10.713014656710872</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.054352903144363</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <f t="shared" ca="1" si="1"/>
+        <v>-4.994680096814049</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.293094781976583</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.35095477672616454</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.5213185861899916</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <f t="shared" ca="1" si="1"/>
+        <v>-10.924677831006086</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.6495068811658404</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <f t="shared" ca="1" si="1"/>
+        <v>-1.0633224468042519</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <f t="shared" ca="1" si="1"/>
+        <v>-6.0194507203596093</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.99937480795590683</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.6459751152037105</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.2431267334129608</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <f t="shared" ca="1" si="1"/>
+        <v>-3.5364504247643551</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.8218040679837424</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.9964892835217869</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <f t="shared" ca="1" si="1"/>
+        <v>-3.9148988501812148</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.4360723482002431</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.56779794269997885</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <f t="shared" ca="1" si="1"/>
+        <v>-11.077746139278236</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <f t="shared" ca="1" si="1"/>
+        <v>-4.1041062121105965</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <f t="shared" ca="1" si="1"/>
+        <v>-4.3647654369046389</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.1483613245179189</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <f t="shared" ca="1" si="1"/>
+        <v>-1.5487987922835607</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <f t="shared" ca="1" si="1"/>
+        <v>-5.3391450698388176</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.4978397442485454</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.79172798527421251</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <f t="shared" ca="1" si="1"/>
+        <v>-4.1337241103549944</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <f t="shared" ca="1" si="1"/>
+        <v>-2.5587749544685279</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.192499773159625</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <f t="shared" ca="1" si="1"/>
+        <v>-1.9941394084354791</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.666405491297672</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <f t="shared" ca="1" si="1"/>
+        <v>-9.0370072905326584</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <f t="shared" ca="1" si="1"/>
+        <v>-1.2026084552916763</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <f t="shared" ca="1" si="1"/>
+        <v>-2.102105919689286</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <f t="shared" ca="1" si="1"/>
+        <v>-6.670671047875917</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.12795845613454734</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <f t="shared" ca="1" si="1"/>
+        <v>6.0613703608163449</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <f t="shared" ca="1" si="1"/>
+        <v>-3.9545660855137066</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <f t="shared" ca="1" si="1"/>
+        <v>6.5229750848002759</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.852719168659493</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <f t="shared" ca="1" si="1"/>
+        <v>-3.8549784352769487</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <f t="shared" ca="1" si="1"/>
+        <v>10.239299352487961</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <f t="shared" ca="1" si="1"/>
+        <v>-6.5442518270630554</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <f t="shared" ca="1" si="1"/>
+        <v>-1.1099496345838209</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.1603261139354704</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <f t="shared" ref="A130:A193" ca="1" si="2">_xlfn.NORM.INV(RAND(),0,5)</f>
+        <v>4.3234608807632791</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <f t="shared" ca="1" si="2"/>
+        <v>3.5332932632904517</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.3371882087455482</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.9547496855519055</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.39752731126786789</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.41887725127272391</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <f t="shared" ca="1" si="2"/>
+        <v>8.0993045191899036</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.2924397817351649</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <f t="shared" ca="1" si="2"/>
+        <v>-3.8111106778514419</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.2845175998863869</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.7204242952880673</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <f t="shared" ca="1" si="2"/>
+        <v>-8.6070430845798818</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.1509311632443646</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.0376529834589692</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <f t="shared" ca="1" si="2"/>
+        <v>10.479597489498522</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.46017286498578142</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <f t="shared" ca="1" si="2"/>
+        <v>-9.071252324866883</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <f t="shared" ca="1" si="2"/>
+        <v>-4.4757334299433076</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.0016772293065004</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.1274056535928154</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.4141908782286357</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.7390279750295123</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.9305838746181647</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.76056870850478808</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.3595283047026805</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <f t="shared" ca="1" si="2"/>
+        <v>-6.9796474163891329</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <f t="shared" ca="1" si="2"/>
+        <v>-4.3371079442570863</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.0470674089709944</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.6868498725502983</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <f t="shared" ca="1" si="2"/>
+        <v>-5.0826472268468548</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.33023000851270295</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.37795166214493997</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <f t="shared" ca="1" si="2"/>
+        <v>-6.8281215699244004</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <f t="shared" ca="1" si="2"/>
+        <v>-2.0543241687755098</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.8233066913947287</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <f t="shared" ca="1" si="2"/>
+        <v>-5.306996552699208</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <f t="shared" ca="1" si="2"/>
+        <v>-9.4487634642269764</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.97517248553454017</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.1193390197090647</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.9085260895208971</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.23435975320425048</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <f t="shared" ca="1" si="2"/>
+        <v>-8.5339928886612011</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.63467962284647184</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.1890119483860917</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <f t="shared" ca="1" si="2"/>
+        <v>-2.3064136413859178</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.38731326379183</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <f t="shared" ca="1" si="2"/>
+        <v>-2.0206851941103867</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.3779937690832949</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.58080043663942282</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <f t="shared" ca="1" si="2"/>
+        <v>-6.8076571272558049</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.4711791075083516</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <f t="shared" ca="1" si="2"/>
+        <v>9.3331935835978541</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <f t="shared" ca="1" si="2"/>
+        <v>0.51963252143786043</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.6604042639288359</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.0530983014567514</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4171514944164727</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <f t="shared" ca="1" si="2"/>
+        <v>-3.0561524188587708</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.7460579406564112</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <f t="shared" ca="1" si="2"/>
+        <v>3.2532592120511854</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.634024350277238</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.29463066868742011</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <f t="shared" ca="1" si="2"/>
+        <v>8.8141136371769075</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <f t="shared" ca="1" si="2"/>
+        <v>-8.1570828531618636E-2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <f t="shared" ca="1" si="2"/>
+        <v>3.3179023290806793</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <f t="shared" ref="A194:A257" ca="1" si="3">_xlfn.NORM.INV(RAND(),0,5)</f>
+        <v>0.22781895430783658</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <f t="shared" ca="1" si="3"/>
+        <v>-4.0455433660547122</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <f t="shared" ca="1" si="3"/>
+        <v>-4.5156820350455318</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <f t="shared" ca="1" si="3"/>
+        <v>-6.8144062685524478</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <f t="shared" ca="1" si="3"/>
+        <v>7.4180320712084447</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <f t="shared" ca="1" si="3"/>
+        <v>-5.2509965153497546</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <f t="shared" ca="1" si="3"/>
+        <v>-2.8100361831289544</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <f t="shared" ca="1" si="3"/>
+        <v>-6.3186489029941839</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <f t="shared" ca="1" si="3"/>
+        <v>10.238839312388686</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <f t="shared" ca="1" si="3"/>
+        <v>9.1517536585802226</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.40611574191196698</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <f t="shared" ca="1" si="3"/>
+        <v>5.2536052363080712</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <f t="shared" ca="1" si="3"/>
+        <v>-3.6660840736204858</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <f t="shared" ca="1" si="3"/>
+        <v>-3.7642447859296428</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <f t="shared" ca="1" si="3"/>
+        <v>12.979797560492406</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <f t="shared" ca="1" si="3"/>
+        <v>-2.889732080014245</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <f t="shared" ca="1" si="3"/>
+        <v>3.5519375454644386</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.39286652500684904</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <f t="shared" ca="1" si="3"/>
+        <v>-6.9473841540949568</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <f t="shared" ca="1" si="3"/>
+        <v>-1.1752017444329286</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <f t="shared" ca="1" si="3"/>
+        <v>10.844690345505787</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <f t="shared" ca="1" si="3"/>
+        <v>1.901076380991948</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <f t="shared" ca="1" si="3"/>
+        <v>-1.5428211093732236</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <f t="shared" ca="1" si="3"/>
+        <v>-9.7271160066166331</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <f t="shared" ca="1" si="3"/>
+        <v>-6.1412739675625891</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <f t="shared" ca="1" si="3"/>
+        <v>-7.0364777861622709</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.27825781297552465</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.18015943397525447</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <f t="shared" ca="1" si="3"/>
+        <v>-1.546077586379158</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <f t="shared" ca="1" si="3"/>
+        <v>-1.6410939577317532</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.49827939029214668</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <f t="shared" ca="1" si="3"/>
+        <v>4.8589499148471438</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <f t="shared" ca="1" si="3"/>
+        <v>-6.1411895841610136</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <f t="shared" ca="1" si="3"/>
+        <v>6.7054178762601584</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <f t="shared" ca="1" si="3"/>
+        <v>10.170818173110982</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <f t="shared" ca="1" si="3"/>
+        <v>3.8955320768561275</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <f t="shared" ca="1" si="3"/>
+        <v>-9.9081800663719584</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <f t="shared" ca="1" si="3"/>
+        <v>-1.5637882177966367</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A232">
+        <f t="shared" ca="1" si="3"/>
+        <v>1.2386323133822881</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A233">
+        <f t="shared" ca="1" si="3"/>
+        <v>-9.4217170356957691</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A234">
+        <f t="shared" ca="1" si="3"/>
+        <v>-2.1240385673466724</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.61326276629075638</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <f t="shared" ca="1" si="3"/>
+        <v>3.1943265057128678</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.61836466123029932</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <f t="shared" ca="1" si="3"/>
+        <v>-7.4022197379204329</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <f t="shared" ca="1" si="3"/>
+        <v>-6.6059007111934607</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <f t="shared" ca="1" si="3"/>
+        <v>6.3386664161457329</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <f t="shared" ca="1" si="3"/>
+        <v>-1.9060225588447808</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.54231883320314023</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <f t="shared" ca="1" si="3"/>
+        <v>-8.4145213703769635</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <f t="shared" ca="1" si="3"/>
+        <v>5.107130921027272</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <f t="shared" ca="1" si="3"/>
+        <v>-1.44612584063186</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <f t="shared" ca="1" si="3"/>
+        <v>-1.5004379052833394</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <f t="shared" ca="1" si="3"/>
+        <v>4.9279489439208817</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <f t="shared" ca="1" si="3"/>
+        <v>9.2732582834773911</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <f t="shared" ca="1" si="3"/>
+        <v>3.5124508033532615</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <f t="shared" ca="1" si="3"/>
+        <v>2.7300634988347809</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <f t="shared" ca="1" si="3"/>
+        <v>5.041943662178701</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.37768513237779999</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <f t="shared" ca="1" si="3"/>
+        <v>-2.2158432988067336</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <f t="shared" ca="1" si="3"/>
+        <v>-7.2448617347258439</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <f t="shared" ca="1" si="3"/>
+        <v>-9.288390640200646</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <f t="shared" ca="1" si="3"/>
+        <v>7.5551754522107277</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.67296054861464127</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <f t="shared" ref="A258:A321" ca="1" si="4">_xlfn.NORM.INV(RAND(),0,5)</f>
+        <v>7.002908266579988</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A259">
+        <f t="shared" ca="1" si="4"/>
+        <v>-4.8834544354936851E-2</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <f t="shared" ca="1" si="4"/>
+        <v>-4.0297215828284791</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <f t="shared" ca="1" si="4"/>
+        <v>-2.5667783322911797</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <f t="shared" ca="1" si="4"/>
+        <v>9.332553338682068</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A263">
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.23088415948148755</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A264">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.4013911867305029</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.46475129104521062</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A266">
+        <f t="shared" ca="1" si="4"/>
+        <v>-3.4739022553113537</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A267">
+        <f t="shared" ca="1" si="4"/>
+        <v>8.6638080480308837</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A268">
+        <f t="shared" ca="1" si="4"/>
+        <v>7.3217632779612689</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A269">
+        <f t="shared" ca="1" si="4"/>
+        <v>-3.2374777507396475</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A270">
+        <f t="shared" ca="1" si="4"/>
+        <v>4.1530076027869631</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A271">
+        <f t="shared" ca="1" si="4"/>
+        <v>-3.2308434833885475</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A272">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.9802012790983037</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A273">
+        <f t="shared" ca="1" si="4"/>
+        <v>4.2834487626626094</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <f t="shared" ca="1" si="4"/>
+        <v>8.2607674013739611</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <f t="shared" ca="1" si="4"/>
+        <v>-4.2260221015699484</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A276">
+        <f t="shared" ca="1" si="4"/>
+        <v>-5.965831183776177</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A277">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.1702884355396863</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A278">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.1140381585664096</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A279">
+        <f t="shared" ca="1" si="4"/>
+        <v>4.1987792697987816</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A280">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.62983111074955511</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A281">
+        <f t="shared" ca="1" si="4"/>
+        <v>-6.1006149156104508</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A282">
+        <f t="shared" ca="1" si="4"/>
+        <v>-3.8458829870848064</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A283">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.7396761584723817</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A284">
+        <f t="shared" ca="1" si="4"/>
+        <v>-13.089922330935044</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A285">
+        <f t="shared" ca="1" si="4"/>
+        <v>-5.3928213193804595</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A286">
+        <f t="shared" ca="1" si="4"/>
+        <v>5.8214444579057654</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A287">
+        <f t="shared" ca="1" si="4"/>
+        <v>4.8510102907681878</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A288">
+        <f t="shared" ca="1" si="4"/>
+        <v>-8.3968901081674971</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A289">
+        <f t="shared" ca="1" si="4"/>
+        <v>-5.6203938306877452</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A290">
+        <f t="shared" ca="1" si="4"/>
+        <v>4.1718821091194158</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A291">
+        <f t="shared" ca="1" si="4"/>
+        <v>-2.7746778997506034</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A292">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.2717280429187561</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A293">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.81482518526321779</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A294">
+        <f t="shared" ca="1" si="4"/>
+        <v>-3.5204432996047403</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A295">
+        <f t="shared" ca="1" si="4"/>
+        <v>8.1551326890283278</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A296">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.6685785513415348</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A297">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.64200886205344576</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A298">
+        <f t="shared" ca="1" si="4"/>
+        <v>-4.5479663927572584</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A299">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.7985245395476512</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A300">
+        <f t="shared" ca="1" si="4"/>
+        <v>-1.1150438448996849</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A301">
+        <f t="shared" ca="1" si="4"/>
+        <v>-3.5259437942901779</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A302">
+        <f t="shared" ca="1" si="4"/>
+        <v>6.0017519232181886</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A303">
+        <f t="shared" ca="1" si="4"/>
+        <v>-6.8511851749145141</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A304">
+        <f t="shared" ca="1" si="4"/>
+        <v>-7.9476316156208826</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A305">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.7593098397084395</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A306">
+        <f t="shared" ca="1" si="4"/>
+        <v>4.2125873730284642</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A307">
+        <f t="shared" ca="1" si="4"/>
+        <v>-9.3982088123897363</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A308">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.662571138117185</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A309">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.462435310990446</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A310">
+        <f t="shared" ca="1" si="4"/>
+        <v>2.933243256414376</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A311">
+        <f t="shared" ca="1" si="4"/>
+        <v>-7.2752447692077826</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A312">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.2647553857336482</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A313">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.7401189894027291</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A314">
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.44624805180822724</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A315">
+        <f t="shared" ca="1" si="4"/>
+        <v>3.5523055289984615</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A316">
+        <f t="shared" ca="1" si="4"/>
+        <v>7.3618475246115196</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A317">
+        <f t="shared" ca="1" si="4"/>
+        <v>6.7275657829780489</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A318">
+        <f t="shared" ca="1" si="4"/>
+        <v>-8.4759939520074372</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A319">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.36968124007835357</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A320">
+        <f t="shared" ca="1" si="4"/>
+        <v>-8.4741814723157329</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A321">
+        <f t="shared" ca="1" si="4"/>
+        <v>6.6802569881831095</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A322">
+        <f t="shared" ref="A322:A385" ca="1" si="5">_xlfn.NORM.INV(RAND(),0,5)</f>
+        <v>7.0696836048942613</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A323">
+        <f t="shared" ca="1" si="5"/>
+        <v>-0.22786276972071157</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A324">
+        <f t="shared" ca="1" si="5"/>
+        <v>4.695732165505099</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A325">
+        <f t="shared" ca="1" si="5"/>
+        <v>6.7875082714658515</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A326">
+        <f t="shared" ca="1" si="5"/>
+        <v>4.5325671490661499</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A327">
+        <f t="shared" ca="1" si="5"/>
+        <v>2.3907640392988174</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A328">
+        <f t="shared" ca="1" si="5"/>
+        <v>-2.6126611741242201</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A329">
+        <f t="shared" ca="1" si="5"/>
+        <v>-1.6720744457667867</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A330">
+        <f t="shared" ca="1" si="5"/>
+        <v>-1.1957862117001508</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A331">
+        <f t="shared" ca="1" si="5"/>
+        <v>-1.9388725243339653</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A332">
+        <f t="shared" ca="1" si="5"/>
+        <v>2.2046791649424171</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A333">
+        <f t="shared" ca="1" si="5"/>
+        <v>-2.2907205040839536</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A334">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.1420611252741142</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A335">
+        <f t="shared" ca="1" si="5"/>
+        <v>8.7984523619718651</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A336">
+        <f t="shared" ca="1" si="5"/>
+        <v>-10.421424485368334</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A337">
+        <f t="shared" ca="1" si="5"/>
+        <v>5.3130922801312286</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A338">
+        <f t="shared" ca="1" si="5"/>
+        <v>-0.89932894248960094</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A339">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.10266283847804109</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A340">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.95174072354403316</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A341">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.6887043884438633</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A342">
+        <f t="shared" ca="1" si="5"/>
+        <v>-7.6916667105823064</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A343">
+        <f t="shared" ca="1" si="5"/>
+        <v>-3.9364985468905149</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A344">
+        <f t="shared" ca="1" si="5"/>
+        <v>10.211082044361628</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A345">
+        <f t="shared" ca="1" si="5"/>
+        <v>-1.1680819258247497</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A346">
+        <f t="shared" ca="1" si="5"/>
+        <v>5.2053513425167708</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A347">
+        <f t="shared" ca="1" si="5"/>
+        <v>-2.7161197677243547</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A348">
+        <f t="shared" ca="1" si="5"/>
+        <v>-4.8556303151757838</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A349">
+        <f t="shared" ca="1" si="5"/>
+        <v>10.772328134875636</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A350">
+        <f t="shared" ca="1" si="5"/>
+        <v>-3.8498570649749055</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A351">
+        <f t="shared" ca="1" si="5"/>
+        <v>-5.8483088664968488</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A352">
+        <f t="shared" ca="1" si="5"/>
+        <v>-4.9065743788206548</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A353">
+        <f t="shared" ca="1" si="5"/>
+        <v>-4.9000498328359132</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A354">
+        <f t="shared" ca="1" si="5"/>
+        <v>-1.4997984172201009</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A355">
+        <f t="shared" ca="1" si="5"/>
+        <v>8.3496351450967374</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A356">
+        <f t="shared" ca="1" si="5"/>
+        <v>-2.3035443699827733</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A357">
+        <f t="shared" ca="1" si="5"/>
+        <v>-1.7240637826852092</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A358">
+        <f t="shared" ca="1" si="5"/>
+        <v>-2.6076049844958646</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A359">
+        <f t="shared" ca="1" si="5"/>
+        <v>-7.7822966091998849</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A360">
+        <f t="shared" ca="1" si="5"/>
+        <v>2.8198856835031334</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A361">
+        <f t="shared" ca="1" si="5"/>
+        <v>5.3731431386449806</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A362">
+        <f t="shared" ca="1" si="5"/>
+        <v>-2.7556829826783673</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A363">
+        <f t="shared" ca="1" si="5"/>
+        <v>-5.3226681980104642</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A364">
+        <f t="shared" ca="1" si="5"/>
+        <v>-0.31252578141747583</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A365">
+        <f t="shared" ca="1" si="5"/>
+        <v>5.2658266503374627</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A366">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.57328569756788872</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A367">
+        <f t="shared" ca="1" si="5"/>
+        <v>-8.414544893198233</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A368">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.69996699745752577</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A369">
+        <f t="shared" ca="1" si="5"/>
+        <v>-2.852177640210749</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A370">
+        <f t="shared" ca="1" si="5"/>
+        <v>-2.3460649759765451</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A371">
+        <f t="shared" ca="1" si="5"/>
+        <v>-4.2784400159424365</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A372">
+        <f t="shared" ca="1" si="5"/>
+        <v>1.1141463095043855</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A373">
+        <f t="shared" ca="1" si="5"/>
+        <v>-0.14377109095386376</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A374">
+        <f t="shared" ca="1" si="5"/>
+        <v>-7.9628467197035793</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A375">
+        <f t="shared" ca="1" si="5"/>
+        <v>-5.1199911645439879</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A376">
+        <f t="shared" ca="1" si="5"/>
+        <v>-6.0665219561759685</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A377">
+        <f t="shared" ca="1" si="5"/>
+        <v>-8.9602179192389322</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A378">
+        <f t="shared" ca="1" si="5"/>
+        <v>-8.3418404196981726</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A379">
+        <f t="shared" ca="1" si="5"/>
+        <v>-0.68869250518288794</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A380">
+        <f t="shared" ca="1" si="5"/>
+        <v>5.7962195357295085</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A381">
+        <f t="shared" ca="1" si="5"/>
+        <v>-5.8923108840050862</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A382">
+        <f t="shared" ca="1" si="5"/>
+        <v>9.3893292026807593</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A383">
+        <f t="shared" ca="1" si="5"/>
+        <v>4.4918180486644985</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A384">
+        <f t="shared" ca="1" si="5"/>
+        <v>-5.2023415240330442</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A385">
+        <f t="shared" ca="1" si="5"/>
+        <v>-0.46217180224810134</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A386">
+        <f t="shared" ref="A386:A449" ca="1" si="6">_xlfn.NORM.INV(RAND(),0,5)</f>
+        <v>2.4135857998344572</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A387">
+        <f t="shared" ca="1" si="6"/>
+        <v>-1.6258026843492115</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A388">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.28903926425930698</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A389">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.6999870962150192</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A390">
+        <f t="shared" ca="1" si="6"/>
+        <v>5.8753625442784934</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A391">
+        <f t="shared" ca="1" si="6"/>
+        <v>6.1391031329768317</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A392">
+        <f t="shared" ca="1" si="6"/>
+        <v>-1.6146146850663299</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A393">
+        <f t="shared" ca="1" si="6"/>
+        <v>2.6417187456672977</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A394">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.4365778681175489</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A395">
+        <f t="shared" ca="1" si="6"/>
+        <v>-1.0936252239388251</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A396">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.21930904566201231</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A397">
+        <f t="shared" ca="1" si="6"/>
+        <v>-7.8229234469068381</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A398">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.4340654425409296</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A399">
+        <f t="shared" ca="1" si="6"/>
+        <v>-3.9750024669604009</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A400">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.0092486343513523</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A401">
+        <f t="shared" ca="1" si="6"/>
+        <v>2.867416400115486</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A402">
+        <f t="shared" ca="1" si="6"/>
+        <v>-6.9730795336157332</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A403">
+        <f t="shared" ca="1" si="6"/>
+        <v>-3.5154744123243304</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A404">
+        <f t="shared" ca="1" si="6"/>
+        <v>-7.4772436368394164</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A405">
+        <f t="shared" ca="1" si="6"/>
+        <v>2.9224698087046566</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A406">
+        <f t="shared" ca="1" si="6"/>
+        <v>6.7249573369085427</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A407">
+        <f t="shared" ca="1" si="6"/>
+        <v>-5.7391925510631356</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A408">
+        <f t="shared" ca="1" si="6"/>
+        <v>-1.1792795248574262</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A409">
+        <f t="shared" ca="1" si="6"/>
+        <v>5.664462779714202</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A410">
+        <f t="shared" ca="1" si="6"/>
+        <v>11.994792334943092</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A411">
+        <f t="shared" ca="1" si="6"/>
+        <v>13.649425625928014</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A412">
+        <f t="shared" ca="1" si="6"/>
+        <v>8.9772203941444211</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A413">
+        <f t="shared" ca="1" si="6"/>
+        <v>-5.578864477123604</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A414">
+        <f t="shared" ca="1" si="6"/>
+        <v>-1.3479863433379566</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A415">
+        <f t="shared" ca="1" si="6"/>
+        <v>3.9370502102064604</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A416">
+        <f t="shared" ca="1" si="6"/>
+        <v>4.3137170763080146</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A417">
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.6432020817103199</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A418">
+        <f t="shared" ca="1" si="6"/>
+        <v>4.4528913603982883</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A419">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.6586672862556382</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A420">
+        <f t="shared" ca="1" si="6"/>
+        <v>2.0596874509027572</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A421">
+        <f t="shared" ca="1" si="6"/>
+        <v>-3.0339907156977124</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A422">
+        <f t="shared" ca="1" si="6"/>
+        <v>-2.0700808232334649</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A423">
+        <f t="shared" ca="1" si="6"/>
+        <v>8.0421309900271822</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A424">
+        <f t="shared" ca="1" si="6"/>
+        <v>-5.0285782670464698</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A425">
+        <f t="shared" ca="1" si="6"/>
+        <v>0.15542287973500382</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A426">
+        <f t="shared" ca="1" si="6"/>
+        <v>7.2155187539080465</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A427">
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.96852241989951471</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A428">
+        <f t="shared" ca="1" si="6"/>
+        <v>6.1541538756832646</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A429">
+        <f t="shared" ca="1" si="6"/>
+        <v>-5.0697422784124866</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A430">
+        <f t="shared" ca="1" si="6"/>
+        <v>-5.757240289405404</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A431">
+        <f t="shared" ca="1" si="6"/>
+        <v>-7.4172448325460039</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A432">
+        <f t="shared" ca="1" si="6"/>
+        <v>7.1561333901630029</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A433">
+        <f t="shared" ca="1" si="6"/>
+        <v>10.870079055343187</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A434">
+        <f t="shared" ca="1" si="6"/>
+        <v>-7.202628485089825</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A435">
+        <f t="shared" ca="1" si="6"/>
+        <v>8.9227787788731519</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A436">
+        <f t="shared" ca="1" si="6"/>
+        <v>-8.0562149471317372</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A437">
+        <f t="shared" ca="1" si="6"/>
+        <v>-4.6395156575908949</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A438">
+        <f t="shared" ca="1" si="6"/>
+        <v>3.8885199717845733</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A439">
+        <f t="shared" ca="1" si="6"/>
+        <v>11.21459019996848</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A440">
+        <f t="shared" ca="1" si="6"/>
+        <v>-8.1598706395610225</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A441">
+        <f t="shared" ca="1" si="6"/>
+        <v>3.0056253407128612</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A442">
+        <f t="shared" ca="1" si="6"/>
+        <v>4.9967730838443103</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A443">
+        <f t="shared" ca="1" si="6"/>
+        <v>-16.462851022099343</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A444">
+        <f t="shared" ca="1" si="6"/>
+        <v>-3.6040452418742364</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A445">
+        <f t="shared" ca="1" si="6"/>
+        <v>-5.3116863493993804</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A446">
+        <f t="shared" ca="1" si="6"/>
+        <v>-5.9313643709903454</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A447">
+        <f t="shared" ca="1" si="6"/>
+        <v>-2.8663833784662209</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A448">
+        <f t="shared" ca="1" si="6"/>
+        <v>-2.4727609451457329</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A449">
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.10003905448139115</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A450">
+        <f t="shared" ref="A450:A513" ca="1" si="7">_xlfn.NORM.INV(RAND(),0,5)</f>
+        <v>-7.1401977497964166</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A451">
+        <f t="shared" ca="1" si="7"/>
+        <v>1.9905004413015042</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A452">
+        <f t="shared" ca="1" si="7"/>
+        <v>-3.479624219450383</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A453">
+        <f t="shared" ca="1" si="7"/>
+        <v>-1.6976745274967244</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A454">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.80788055421534843</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A455">
+        <f t="shared" ca="1" si="7"/>
+        <v>-9.014531889288687</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A456">
+        <f t="shared" ca="1" si="7"/>
+        <v>-7.8283308596424366</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A457">
+        <f t="shared" ca="1" si="7"/>
+        <v>-1.5681964774737958</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A458">
+        <f t="shared" ca="1" si="7"/>
+        <v>-3.1936215975786104</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A459">
+        <f t="shared" ca="1" si="7"/>
+        <v>5.325454556632482</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A460">
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.42807226878681814</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A461">
+        <f t="shared" ca="1" si="7"/>
+        <v>1.8458901400025618</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A462">
+        <f t="shared" ca="1" si="7"/>
+        <v>-4.7171440020168411</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A463">
+        <f t="shared" ca="1" si="7"/>
+        <v>4.7025668407243044</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A464">
+        <f t="shared" ca="1" si="7"/>
+        <v>-1.2716916948080768</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A465">
+        <f t="shared" ca="1" si="7"/>
+        <v>-4.6387841752769727</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A466">
+        <f t="shared" ca="1" si="7"/>
+        <v>-6.9902417873775438</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A467">
+        <f t="shared" ca="1" si="7"/>
+        <v>2.5425089588752869</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A468">
+        <f t="shared" ca="1" si="7"/>
+        <v>1.2516509073300728</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A469">
+        <f t="shared" ca="1" si="7"/>
+        <v>4.5937927030012053</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A470">
+        <f t="shared" ca="1" si="7"/>
+        <v>-3.1024428232949082</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A471">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.86369306919010036</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A472">
+        <f t="shared" ca="1" si="7"/>
+        <v>2.5866809324608937</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A473">
+        <f t="shared" ca="1" si="7"/>
+        <v>-6.0209333587080138</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A474">
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.27722980862128566</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A475">
+        <f t="shared" ca="1" si="7"/>
+        <v>-8.0468186943784588</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A476">
+        <f t="shared" ca="1" si="7"/>
+        <v>-1.4371086096195997</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A477">
+        <f t="shared" ca="1" si="7"/>
+        <v>-5.308680378260707</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A478">
+        <f t="shared" ca="1" si="7"/>
+        <v>-10.292647720487572</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A479">
+        <f t="shared" ca="1" si="7"/>
+        <v>-2.6262766910286475</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A480">
+        <f t="shared" ca="1" si="7"/>
+        <v>2.3770774197144151</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A481">
+        <f t="shared" ca="1" si="7"/>
+        <v>12.311705444866963</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A482">
+        <f t="shared" ca="1" si="7"/>
+        <v>-6.5259070075543288</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A483">
+        <f t="shared" ca="1" si="7"/>
+        <v>2.4395684847909123</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A484">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.11495595056876128</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A485">
+        <f t="shared" ca="1" si="7"/>
+        <v>5.1798152958580719</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A486">
+        <f t="shared" ca="1" si="7"/>
+        <v>-7.9652313768595153</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A487">
+        <f t="shared" ca="1" si="7"/>
+        <v>-4.3921742170312301</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A488">
+        <f t="shared" ca="1" si="7"/>
+        <v>5.9210122259856002</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A489">
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.35084820600720845</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A490">
+        <f t="shared" ca="1" si="7"/>
+        <v>-2.8116096673729545</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A491">
+        <f t="shared" ca="1" si="7"/>
+        <v>-2.1176778345783909</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A492">
+        <f t="shared" ca="1" si="7"/>
+        <v>2.4448694947887168</v>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A493">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.89096623488102722</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A494">
+        <f t="shared" ca="1" si="7"/>
+        <v>-3.3585324782212371</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A495">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.21465074515180846</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A496">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.50783955446238405</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A497">
+        <f t="shared" ca="1" si="7"/>
+        <v>-6.5413254127505702</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A498">
+        <f t="shared" ca="1" si="7"/>
+        <v>-6.5177447228588337</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A499">
+        <f t="shared" ca="1" si="7"/>
+        <v>1.7473578982580213</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A500">
+        <f t="shared" ca="1" si="7"/>
+        <v>2.4585230388657733</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A501">
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.1526964733737346</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A502">
+        <f t="shared" ca="1" si="7"/>
+        <v>-11.252158702809492</v>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A503">
+        <f t="shared" ca="1" si="7"/>
+        <v>1.3443139667035944</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A504">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.78031047777133677</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A505">
+        <f t="shared" ca="1" si="7"/>
+        <v>1.2392907285345338</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A506">
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.63900031337574248</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A507">
+        <f t="shared" ca="1" si="7"/>
+        <v>0.18601384486627071</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A508">
+        <f t="shared" ca="1" si="7"/>
+        <v>1.99034456899956</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A509">
+        <f t="shared" ca="1" si="7"/>
+        <v>-4.6431973731463341</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A510">
+        <f t="shared" ca="1" si="7"/>
+        <v>-3.5018323382623215</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A511">
+        <f t="shared" ca="1" si="7"/>
+        <v>4.8282279220713722</v>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A512">
+        <f t="shared" ca="1" si="7"/>
+        <v>2.4334307243821192</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A513">
+        <f t="shared" ca="1" si="7"/>
+        <v>5.9679346721649189</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A514">
+        <f t="shared" ref="A514:A577" ca="1" si="8">_xlfn.NORM.INV(RAND(),0,5)</f>
+        <v>-5.3146924070399653</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A515">
+        <f t="shared" ca="1" si="8"/>
+        <v>-3.6923307947383672</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A516">
+        <f t="shared" ca="1" si="8"/>
+        <v>2.6530034705989087</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A517">
+        <f t="shared" ca="1" si="8"/>
+        <v>-3.8008133368043446</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A518">
+        <f t="shared" ca="1" si="8"/>
+        <v>3.3310407501558381</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A519">
+        <f t="shared" ca="1" si="8"/>
+        <v>-6.8071010494945199</v>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A520">
+        <f t="shared" ca="1" si="8"/>
+        <v>8.9792399588110499</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A521">
+        <f t="shared" ca="1" si="8"/>
+        <v>-5.6465054347854533</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A522">
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.12336847346576869</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A523">
+        <f t="shared" ca="1" si="8"/>
+        <v>-2.0799219327010428</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A524">
+        <f t="shared" ca="1" si="8"/>
+        <v>-4.9440794839338658</v>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A525">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.65608028721503131</v>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A526">
+        <f t="shared" ca="1" si="8"/>
+        <v>-3.0114611128676216</v>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A527">
+        <f t="shared" ca="1" si="8"/>
+        <v>7.4466331142577433E-2</v>
+      </c>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A528">
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.66429398533948048</v>
+      </c>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A529">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.81759610768005575</v>
+      </c>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A530">
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.91428681840038051</v>
+      </c>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A531">
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.92331443606348029</v>
+      </c>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A532">
+        <f t="shared" ca="1" si="8"/>
+        <v>2.2755928417779367</v>
+      </c>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A533">
+        <f t="shared" ca="1" si="8"/>
+        <v>6.0642324793116389</v>
+      </c>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A534">
+        <f t="shared" ca="1" si="8"/>
+        <v>3.9709342039026705</v>
+      </c>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A535">
+        <f t="shared" ca="1" si="8"/>
+        <v>-4.0683667322550505</v>
+      </c>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A536">
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.16925117390153091</v>
+      </c>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A537">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.76693251897196557</v>
+      </c>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A538">
+        <f t="shared" ca="1" si="8"/>
+        <v>-3.3586325275347386</v>
+      </c>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A539">
+        <f t="shared" ca="1" si="8"/>
+        <v>9.4351617076461487</v>
+      </c>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A540">
+        <f t="shared" ca="1" si="8"/>
+        <v>3.5503965201579533</v>
+      </c>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A541">
+        <f t="shared" ca="1" si="8"/>
+        <v>-2.232397865849014</v>
+      </c>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A542">
+        <f t="shared" ca="1" si="8"/>
+        <v>3.9377409261652216</v>
+      </c>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A543">
+        <f t="shared" ca="1" si="8"/>
+        <v>5.3507409401554318</v>
+      </c>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A544">
+        <f t="shared" ca="1" si="8"/>
+        <v>14.091204563457138</v>
+      </c>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A545">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.76800369548213687</v>
+      </c>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A546">
+        <f t="shared" ca="1" si="8"/>
+        <v>1.448424540337353</v>
+      </c>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A547">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.33615372373714836</v>
+      </c>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A548">
+        <f t="shared" ca="1" si="8"/>
+        <v>2.2972299768833691</v>
+      </c>
+    </row>
+    <row r="549" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A549">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.52680509643311146</v>
+      </c>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A550">
+        <f t="shared" ca="1" si="8"/>
+        <v>-3.7977695629041945</v>
+      </c>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A551">
+        <f t="shared" ca="1" si="8"/>
+        <v>1.5427848809621827</v>
+      </c>
+    </row>
+    <row r="552" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A552">
+        <f t="shared" ca="1" si="8"/>
+        <v>-3.7552638171786734</v>
+      </c>
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A553">
+        <f t="shared" ca="1" si="8"/>
+        <v>-3.9250331314772269</v>
+      </c>
+    </row>
+    <row r="554" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A554">
+        <f t="shared" ca="1" si="8"/>
+        <v>-4.1510117466016521</v>
+      </c>
+    </row>
+    <row r="555" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A555">
+        <f t="shared" ca="1" si="8"/>
+        <v>-14.546542944179199</v>
+      </c>
+    </row>
+    <row r="556" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A556">
+        <f t="shared" ca="1" si="8"/>
+        <v>5.6496588594871797</v>
+      </c>
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A557">
+        <f t="shared" ca="1" si="8"/>
+        <v>-5.525945293104173</v>
+      </c>
+    </row>
+    <row r="558" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A558">
+        <f t="shared" ca="1" si="8"/>
+        <v>1.9540040629607156</v>
+      </c>
+    </row>
+    <row r="559" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A559">
+        <f t="shared" ca="1" si="8"/>
+        <v>5.712409104749292</v>
+      </c>
+    </row>
+    <row r="560" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A560">
+        <f t="shared" ca="1" si="8"/>
+        <v>-9.9430622333799299</v>
+      </c>
+    </row>
+    <row r="561" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A561">
+        <f t="shared" ca="1" si="8"/>
+        <v>-9.8976169077485547</v>
+      </c>
+    </row>
+    <row r="562" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A562">
+        <f t="shared" ca="1" si="8"/>
+        <v>-3.8372889351139601</v>
+      </c>
+    </row>
+    <row r="563" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A563">
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.46999715868846592</v>
+      </c>
+    </row>
+    <row r="564" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A564">
+        <f t="shared" ca="1" si="8"/>
+        <v>1.7202056349609653</v>
+      </c>
+    </row>
+    <row r="565" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A565">
+        <f t="shared" ca="1" si="8"/>
+        <v>3.7850660679503951</v>
+      </c>
+    </row>
+    <row r="566" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A566">
+        <f t="shared" ca="1" si="8"/>
+        <v>4.3434091235147747</v>
+      </c>
+    </row>
+    <row r="567" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A567">
+        <f t="shared" ca="1" si="8"/>
+        <v>-3.9847090563882515</v>
+      </c>
+    </row>
+    <row r="568" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A568">
+        <f t="shared" ca="1" si="8"/>
+        <v>0.42689767146267987</v>
+      </c>
+    </row>
+    <row r="569" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A569">
+        <f t="shared" ca="1" si="8"/>
+        <v>-3.4834367792555843</v>
+      </c>
+    </row>
+    <row r="570" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A570">
+        <f t="shared" ca="1" si="8"/>
+        <v>-2.6554215605549625</v>
+      </c>
+    </row>
+    <row r="571" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A571">
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.52180595329890411</v>
+      </c>
+    </row>
+    <row r="572" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A572">
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.80108282424325505</v>
+      </c>
+    </row>
+    <row r="573" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A573">
+        <f t="shared" ca="1" si="8"/>
+        <v>-2.5201846168511999</v>
+      </c>
+    </row>
+    <row r="574" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A574">
+        <f t="shared" ca="1" si="8"/>
+        <v>3.378890499957738</v>
+      </c>
+    </row>
+    <row r="575" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A575">
+        <f t="shared" ca="1" si="8"/>
+        <v>-1.6824766597910004</v>
+      </c>
+    </row>
+    <row r="576" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A576">
+        <f t="shared" ca="1" si="8"/>
+        <v>-13.425186670144997</v>
+      </c>
+    </row>
+    <row r="577" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A577">
+        <f t="shared" ca="1" si="8"/>
+        <v>4.4591581052797036</v>
+      </c>
+    </row>
+    <row r="578" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A578">
+        <f t="shared" ref="A578:A598" ca="1" si="9">_xlfn.NORM.INV(RAND(),0,5)</f>
+        <v>-0.32107438929444376</v>
+      </c>
+    </row>
+    <row r="579" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A579">
+        <f t="shared" ca="1" si="9"/>
+        <v>7.0623658054974907</v>
+      </c>
+    </row>
+    <row r="580" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A580">
+        <f t="shared" ca="1" si="9"/>
+        <v>-1.1869577542529151</v>
+      </c>
+    </row>
+    <row r="581" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A581">
+        <f t="shared" ca="1" si="9"/>
+        <v>3.1965475485178767</v>
+      </c>
+    </row>
+    <row r="582" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A582">
+        <f t="shared" ca="1" si="9"/>
+        <v>-7.1322041363785722</v>
+      </c>
+    </row>
+    <row r="583" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A583">
+        <f t="shared" ca="1" si="9"/>
+        <v>7.5850635066585852</v>
+      </c>
+    </row>
+    <row r="584" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A584">
+        <f t="shared" ca="1" si="9"/>
+        <v>3.3579792933763306</v>
+      </c>
+    </row>
+    <row r="585" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A585">
+        <f t="shared" ca="1" si="9"/>
+        <v>2.8656380183570347</v>
+      </c>
+    </row>
+    <row r="586" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A586">
+        <f t="shared" ca="1" si="9"/>
+        <v>1.1643153117039551</v>
+      </c>
+    </row>
+    <row r="587" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A587">
+        <f t="shared" ca="1" si="9"/>
+        <v>-3.7686340803578613</v>
+      </c>
+    </row>
+    <row r="588" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A588">
+        <f t="shared" ca="1" si="9"/>
+        <v>1.8674672274000448</v>
+      </c>
+    </row>
+    <row r="589" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A589">
+        <f t="shared" ca="1" si="9"/>
+        <v>4.728827790981736</v>
+      </c>
+    </row>
+    <row r="590" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A590">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.47845085875773735</v>
+      </c>
+    </row>
+    <row r="591" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A591">
+        <f t="shared" ca="1" si="9"/>
+        <v>0.67636186418157274</v>
+      </c>
+    </row>
+    <row r="592" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A592">
+        <f t="shared" ca="1" si="9"/>
+        <v>-3.3779664298877439</v>
+      </c>
+    </row>
+    <row r="593" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A593">
+        <f t="shared" ca="1" si="9"/>
+        <v>-6.4242740931867273</v>
+      </c>
+    </row>
+    <row r="594" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A594">
+        <f t="shared" ca="1" si="9"/>
+        <v>-4.9016917171599044</v>
+      </c>
+    </row>
+    <row r="595" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A595">
+        <f t="shared" ca="1" si="9"/>
+        <v>2.3674537214801727</v>
+      </c>
+    </row>
+    <row r="596" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A596">
+        <f t="shared" ca="1" si="9"/>
+        <v>-4.2519974607619684</v>
+      </c>
+    </row>
+    <row r="597" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A597">
+        <f t="shared" ca="1" si="9"/>
+        <v>2.0054163165409005</v>
+      </c>
+    </row>
+    <row r="598" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A598">
+        <f t="shared" ca="1" si="9"/>
+        <v>3.792744032883796</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>